<commit_message>
cap nhat thong ke
</commit_message>
<xml_diff>
--- a/HomeworkHackerrank/ThongKeDiemCacNhom.xlsx
+++ b/HomeworkHackerrank/ThongKeDiemCacNhom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocLinh\Desktop\PTTKTT\Thiet-Ke-Thuat-Toan\HomeworkHackerrank\code tung nhom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocLinh\Desktop\PTTKTT\Thiet-Ke-Thuat-Toan\HomeworkHackerrank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDEE7C9-04E8-4FEB-89EA-F6289BBD455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66418432-E782-4C45-AF74-03BC9EA998EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Nhóm</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>300/400</t>
-  </si>
-  <si>
-    <t>88.89/400</t>
   </si>
   <si>
     <t>360.32/400</t>
@@ -454,7 +451,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,13 +606,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,7 +620,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -693,13 +690,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>